<commit_message>
Calculated DE and LF relative areas
</commit_message>
<xml_diff>
--- a/Watershed Areas.xlsx
+++ b/Watershed Areas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsono\Documents\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owenl\Documents\R_Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CCB6A1B-2FD0-4CB6-BAD4-7343219FB50B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E220E434-B083-4B5F-A318-1EED0278E7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" xr2:uid="{C4572688-7631-440E-B1AB-5C2E6E53BC0C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C4572688-7631-440E-B1AB-5C2E6E53BC0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,16 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -94,8 +104,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -126,10 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,18 +459,19 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -490,7 +503,7 @@
         <v>124.7357235061266</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -498,11 +511,11 @@
         <v>1031089315.24616</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D16" si="0">CONVERT(C3, "ft^2",  "km^2")</f>
+        <f t="shared" ref="D3:D15" si="0">CONVERT(C3, "ft^2",  "km^2")</f>
         <v>95.791331897886593</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -514,7 +527,7 @@
         <v>28.727860200115515</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -527,7 +540,7 @@
         <v>0.21653140812448754</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -536,7 +549,7 @@
         <v>0.76795427328548471</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -545,7 +558,7 @@
         <v>0.23030980534381149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -557,7 +570,7 @@
         <v>13.56553562990014</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -568,8 +581,12 @@
         <f t="shared" si="0"/>
         <v>10.239252711931245</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <f>C9/C8*100</f>
+        <v>75.47989988218859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -580,8 +597,12 @@
         <f t="shared" si="0"/>
         <v>75.353657439742648</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>C10/C2</f>
+        <v>0.60410646863359496</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -593,7 +614,7 @@
         <v>249.01466330971914</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -606,7 +627,7 @@
         <v>25.120494022018459</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -618,7 +639,7 @@
         <v>2.4391630000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -631,7 +652,7 @@
         <v>22.681331022018458</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -644,7 +665,7 @@
         <v>223.89416928770066</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Fixed Q calculations, created csvs with Q values
</commit_message>
<xml_diff>
--- a/Watershed Areas.xlsx
+++ b/Watershed Areas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owenl\Documents\R_Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojlarson/Documents/Thesis/R_Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E220E434-B083-4B5F-A318-1EED0278E7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331C8360-307A-8048-8686-09B05E54859C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C4572688-7631-440E-B1AB-5C2E6E53BC0C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31000" windowHeight="11980" xr2:uid="{C4572688-7631-440E-B1AB-5C2E6E53BC0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Watershed Areas</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>of FM</t>
+  </si>
+  <si>
+    <t>of MB</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -141,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,22 +462,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5149F5D8-FD24-4232-9150-5A3CE09CB9DB}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -503,7 +509,7 @@
         <v>124.7357235061266</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -515,7 +521,7 @@
         <v>95.791331897886593</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -527,7 +533,7 @@
         <v>28.727860200115515</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -540,7 +546,7 @@
         <v>0.21653140812448754</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -549,7 +555,7 @@
         <v>0.76795427328548471</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -558,7 +564,7 @@
         <v>0.23030980534381149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -570,7 +576,7 @@
         <v>13.56553562990014</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -582,11 +588,14 @@
         <v>10.239252711931245</v>
       </c>
       <c r="F9" s="3">
-        <f>C9/C8*100</f>
-        <v>75.47989988218859</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <f>C9/C8</f>
+        <v>0.75479899882188584</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -601,8 +610,11 @@
         <f>C10/C2</f>
         <v>0.60410646863359496</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -614,7 +626,7 @@
         <v>249.01466330971914</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -627,7 +639,7 @@
         <v>25.120494022018459</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -639,7 +651,7 @@
         <v>2.4391630000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -652,7 +664,7 @@
         <v>22.681331022018458</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>16</v>
       </c>
@@ -665,7 +677,7 @@
         <v>223.89416928770066</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>15</v>
       </c>

</xml_diff>